<commit_message>
remove quotations from names
</commit_message>
<xml_diff>
--- a/square_raw.xlsx
+++ b/square_raw.xlsx
@@ -11,18 +11,19 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Category" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Category Items" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Modifier Option" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Menu" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Setting" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Visibility Setting" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Day Schedule" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Category ModifierGroups" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Category Modifiers" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Modifier Group" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Modifier ModifierOptions" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Allergen" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tag" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Item Modifiers" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Item Modifier Group" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Modifier" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Menu" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Setting" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Visibility Setting" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Day Schedule" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Category ModifierGroups" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Category Modifiers" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Modifier Group" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Modifier ModifierOptions" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Allergen" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tag" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Item Modifiers" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Item Modifier Group" sheetId="17" state="visible" r:id="rId17"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -456,57 +457,57 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>menuName</t>
+          <t>itemName</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>posDisplayName</t>
+          <t>itemPrice</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>menuDescription</t>
+          <t>itemDescription</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>picture</t>
+          <t>itemPicture</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>startTime</t>
+          <t>onlineImage</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>endTime</t>
+          <t>thirdPartyImage</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>genericModifierId</t>
+          <t>kioskItemImage</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>restaurantId</t>
+          <t>calories</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>sortOrder</t>
+          <t>preparationTime</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>settingId</t>
+          <t>stockStatus</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>posButtonColor</t>
+          <t>showOnMenu</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
@@ -19387,7 +19388,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>modifierId</t>
+          <t>modifierGroupId</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -19402,6 +19403,42 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>categoryId</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>modifierId</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>sortOrder</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -19472,7 +19509,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -19505,42 +19542,6 @@
       <c r="D1" s="1" t="inlineStr">
         <is>
           <t>maxLimit</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>allergenName</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>image</t>
         </is>
       </c>
     </row>
@@ -19571,7 +19572,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>tagName</t>
+          <t>allergenName</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -19602,17 +19603,17 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>itemId</t>
+          <t>id</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>modifierId</t>
+          <t>tagName</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>sortOrder</t>
+          <t>image</t>
         </is>
       </c>
     </row>
@@ -19643,6 +19644,42 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>modifierId</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>sortOrder</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>itemId</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>modifierGroupId</t>
         </is>
       </c>
@@ -19679,7 +19716,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Category</t>
+          <t>categoryName</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -26767,7 +26804,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -26783,7 +26820,57 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>type</t>
+          <t>menuName</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>posDisplayName</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>menuDescription</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>picture</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>startTime</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>endTime</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>genericModifierId</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>restaurantId</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>sortOrder</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>settingId</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>posButtonColor</t>
         </is>
       </c>
     </row>
@@ -26798,7 +26885,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -26814,22 +26901,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>isDefault</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>channelVisibilityType</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>device</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>settingId</t>
+          <t>type</t>
         </is>
       </c>
     </row>
@@ -26860,22 +26932,22 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>day</t>
+          <t>isDefault</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>startTime</t>
+          <t>channelVisibilityType</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>endTime</t>
+          <t>device</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>visibilitySettingId</t>
+          <t>settingId</t>
         </is>
       </c>
     </row>
@@ -26890,7 +26962,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -26901,17 +26973,27 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>categoryId</t>
+          <t>id</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>modifierGroupId</t>
+          <t>day</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>sortOrder</t>
+          <t>startTime</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>endTime</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>visibilitySettingId</t>
         </is>
       </c>
     </row>

</xml_diff>